<commit_message>
Adicionando instruções no arquivo Passo a Passo.ipynb sobre o executável main.exe e sua execução
</commit_message>
<xml_diff>
--- a/data/output.xlsx
+++ b/data/output.xlsx
@@ -752,16 +752,16 @@
         <v>22</v>
       </c>
       <c r="D8" s="2">
-        <v>178.9563939924111</v>
+        <v>178.9563786732192</v>
       </c>
       <c r="E8" s="2">
-        <v>179.1849673492164</v>
+        <v>179.184952010458</v>
       </c>
       <c r="F8" s="2">
-        <v>176.2432663098354</v>
+        <v>176.2432512228952</v>
       </c>
       <c r="G8" s="2">
-        <v>178.2507781982422</v>
+        <v>178.2507629394531</v>
       </c>
       <c r="H8" s="2">
         <v>58953100</v>
@@ -782,16 +782,16 @@
         <v>23</v>
       </c>
       <c r="D9" s="2">
-        <v>178.3799448074533</v>
+        <v>178.3799603423375</v>
       </c>
       <c r="E9" s="2">
-        <v>179.0159861039513</v>
+        <v>179.0160016942275</v>
       </c>
       <c r="F9" s="2">
-        <v>173.7388283656852</v>
+        <v>173.7388434963805</v>
       </c>
       <c r="G9" s="2">
-        <v>175.2096710205078</v>
+        <v>175.2096862792969</v>
       </c>
       <c r="H9" s="2">
         <v>90370200</v>
@@ -812,16 +812,16 @@
         <v>24</v>
       </c>
       <c r="D10" s="2">
-        <v>175.4183623155366</v>
+        <v>175.4183777757781</v>
       </c>
       <c r="E10" s="2">
-        <v>176.2034850251751</v>
+        <v>176.2035005546122</v>
       </c>
       <c r="F10" s="2">
-        <v>172.9040104015583</v>
+        <v>172.9040256402011</v>
       </c>
       <c r="G10" s="2">
-        <v>173.1325988769531</v>
+        <v>173.1326141357422</v>
       </c>
       <c r="H10" s="2">
         <v>84267900</v>
@@ -1152,16 +1152,16 @@
         <v>44</v>
       </c>
       <c r="D21" s="2">
-        <v>9.241198173218374</v>
+        <v>9.241199117840845</v>
       </c>
       <c r="E21" s="2">
-        <v>9.355052966541995</v>
+        <v>9.355053922802545</v>
       </c>
       <c r="F21" s="2">
-        <v>9.196921577247355</v>
+        <v>9.196922517343934</v>
       </c>
       <c r="G21" s="2">
-        <v>9.329751968383789</v>
+        <v>9.329752922058105</v>
       </c>
       <c r="H21" s="2">
         <v>19896800</v>
@@ -1182,16 +1182,16 @@
         <v>45</v>
       </c>
       <c r="D22" s="2">
-        <v>9.30445154105194</v>
+        <v>9.304452485099688</v>
       </c>
       <c r="E22" s="2">
-        <v>9.462582940047911</v>
+        <v>9.462583900139981</v>
       </c>
       <c r="F22" s="2">
-        <v>9.29812614031848</v>
+        <v>9.298127083724443</v>
       </c>
       <c r="G22" s="2">
-        <v>9.399330139160156</v>
+        <v>9.399331092834473</v>
       </c>
       <c r="H22" s="2">
         <v>24996900</v>
@@ -1212,16 +1212,16 @@
         <v>46</v>
       </c>
       <c r="D23" s="2">
-        <v>9.601739020590145</v>
+        <v>9.601737960796838</v>
       </c>
       <c r="E23" s="2">
-        <v>9.772520622819153</v>
+        <v>9.772519544175802</v>
       </c>
       <c r="F23" s="2">
-        <v>8.127954387147648</v>
+        <v>8.127953490023529</v>
       </c>
       <c r="G23" s="2">
-        <v>8.640299797058105</v>
+        <v>8.640298843383789</v>
       </c>
       <c r="H23" s="2">
         <v>157468400</v>

</xml_diff>

<commit_message>
Vídeo do Funcionamento do Programa
</commit_message>
<xml_diff>
--- a/data/output.xlsx
+++ b/data/output.xlsx
@@ -130,13 +130,13 @@
     <t>B3SA3.SA</t>
   </si>
   <si>
-    <t>10.37</t>
+    <t>10.38</t>
   </si>
   <si>
     <t>MGLU3.SA</t>
   </si>
   <si>
-    <t>6.37</t>
+    <t>6.43</t>
   </si>
   <si>
     <t>2024-12-20</t>
@@ -782,16 +782,16 @@
         <v>23</v>
       </c>
       <c r="D9" s="2">
-        <v>178.3799603423375</v>
+        <v>178.3799758772218</v>
       </c>
       <c r="E9" s="2">
-        <v>179.0160016942275</v>
+        <v>179.0160172845038</v>
       </c>
       <c r="F9" s="2">
-        <v>173.7388434963805</v>
+        <v>173.7388586270757</v>
       </c>
       <c r="G9" s="2">
-        <v>175.2096862792969</v>
+        <v>175.2097015380859</v>
       </c>
       <c r="H9" s="2">
         <v>90370200</v>
@@ -812,16 +812,16 @@
         <v>24</v>
       </c>
       <c r="D10" s="2">
-        <v>175.4183777757781</v>
+        <v>175.4183932360196</v>
       </c>
       <c r="E10" s="2">
-        <v>176.2035005546122</v>
+        <v>176.2035160840494</v>
       </c>
       <c r="F10" s="2">
-        <v>172.9040256402011</v>
+        <v>172.9040408788438</v>
       </c>
       <c r="G10" s="2">
-        <v>173.1326141357422</v>
+        <v>173.1326293945312</v>
       </c>
       <c r="H10" s="2">
         <v>84267900</v>
@@ -1103,7 +1103,7 @@
         <v>29510200</v>
       </c>
       <c r="I19" s="2">
-        <v>0.063363</v>
+        <v>0.06403399999999999</v>
       </c>
       <c r="J19" s="2">
         <v>0</v>
@@ -1182,16 +1182,16 @@
         <v>45</v>
       </c>
       <c r="D22" s="2">
-        <v>9.304452485099688</v>
+        <v>9.304450597004189</v>
       </c>
       <c r="E22" s="2">
-        <v>9.462583900139981</v>
+        <v>9.462581979955843</v>
       </c>
       <c r="F22" s="2">
-        <v>9.298127083724443</v>
+        <v>9.298125196912519</v>
       </c>
       <c r="G22" s="2">
-        <v>9.399331092834473</v>
+        <v>9.39932918548584</v>
       </c>
       <c r="H22" s="2">
         <v>24996900</v>
@@ -1212,16 +1212,16 @@
         <v>46</v>
       </c>
       <c r="D23" s="2">
-        <v>9.601737960796838</v>
+        <v>9.60173690100353</v>
       </c>
       <c r="E23" s="2">
-        <v>9.772519544175802</v>
+        <v>9.772518465532452</v>
       </c>
       <c r="F23" s="2">
-        <v>8.127953490023529</v>
+        <v>8.12795259289941</v>
       </c>
       <c r="G23" s="2">
-        <v>8.640298843383789</v>
+        <v>8.640297889709473</v>
       </c>
       <c r="H23" s="2">
         <v>157468400</v>

</xml_diff>